<commit_message>
New structure for event changes
</commit_message>
<xml_diff>
--- a/DataSource/excel/cityBuilding.xlsx
+++ b/DataSource/excel/cityBuilding.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujiel/Documents/mygit/SailingGame/DataSource/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="7880" yWindow="1240" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cityBuilding.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -78,40 +86,37 @@
     <t>int</t>
   </si>
   <si>
-    <t>portraitId</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>Bar</t>
-  </si>
-  <si>
-    <t>Square</t>
-  </si>
-  <si>
-    <t>Exchange</t>
-  </si>
-  <si>
-    <t>Shipyard</t>
-  </si>
-  <si>
-    <t>Inn</t>
-  </si>
-  <si>
-    <t>Dock</t>
-  </si>
-  <si>
-    <t>Office</t>
-  </si>
-  <si>
-    <t>Church</t>
-  </si>
-  <si>
-    <t>Outside</t>
-  </si>
-  <si>
     <t>npcNameId</t>
+  </si>
+  <si>
+    <t>eventAction</t>
+  </si>
+  <si>
+    <t>government</t>
+  </si>
+  <si>
+    <t>plaza</t>
+  </si>
+  <si>
+    <t>exchange</t>
+  </si>
+  <si>
+    <t>shipyard</t>
+  </si>
+  <si>
+    <t>inn</t>
+  </si>
+  <si>
+    <t>dock</t>
+  </si>
+  <si>
+    <t>shop</t>
+  </si>
+  <si>
+    <t>relic</t>
+  </si>
+  <si>
+    <t>tarven</t>
   </si>
 </sst>
 </file>
@@ -191,6 +196,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -519,15 +529,15 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -538,13 +548,13 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -561,7 +571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -575,10 +585,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -592,10 +602,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -609,10 +619,10 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -629,7 +639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -646,7 +656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -663,12 +673,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -677,10 +687,10 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -697,12 +707,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -711,10 +721,10 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -728,10 +738,10 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -745,10 +755,10 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -768,10 +778,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove unused class, and minor fix
</commit_message>
<xml_diff>
--- a/DataSource/excel/cityBuilding.xlsx
+++ b/DataSource/excel/cityBuilding.xlsx
@@ -116,7 +116,7 @@
     <t>relic</t>
   </si>
   <si>
-    <t>tarven</t>
+    <t>tavern</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>